<commit_message>
added pheno file gen for gemma and data tranformations
</commit_message>
<xml_diff>
--- a/Radish_Phenotype_Data.xlsx
+++ b/Radish_Phenotype_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bakhtiar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliaharencar/Documents/Github/Raphanus_color_chem_GWAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F7F705-6F61-474E-A827-F5F11F04871E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72E1935-D151-5E44-86E5-7BB5E68B1A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="1485" windowWidth="21045" windowHeight="13380" xr2:uid="{B8EC26B0-6085-4EB8-8ACA-F429418B303E}"/>
+    <workbookView xWindow="4940" yWindow="1480" windowWidth="21040" windowHeight="13380" xr2:uid="{B8EC26B0-6085-4EB8-8ACA-F429418B303E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -187,9 +187,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -227,7 +227,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -333,7 +333,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -475,7 +475,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -486,26 +486,26 @@
   <dimension ref="A1:L385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="I9" activeCellId="1" sqref="E29 I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.1640625" style="3"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -543,7 +543,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -581,7 +581,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1.1000000000000001</v>
       </c>
@@ -619,7 +619,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2.1</v>
       </c>
@@ -657,7 +657,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2.2000000000000002</v>
       </c>
@@ -695,7 +695,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>2.2000000000000002</v>
       </c>
@@ -733,7 +733,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>3.2</v>
       </c>
@@ -771,7 +771,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>3.2</v>
       </c>
@@ -809,7 +809,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>5.0999999999999996</v>
       </c>
@@ -847,7 +847,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>6.2</v>
       </c>
@@ -885,7 +885,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>6.2</v>
       </c>
@@ -923,7 +923,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>8.1</v>
       </c>
@@ -961,7 +961,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>8.1</v>
       </c>
@@ -999,7 +999,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>8.3000000000000007</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>8.4</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>8.4</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>11.2</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>11.2</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>13.2</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>13.2</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>16.2</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>16.2</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>18.2</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>18.2</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>19.100000000000001</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>19.100000000000001</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>23.2</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>23.2</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>24.1</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>25.2</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>25.2</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>27.3</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>27.3</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>28.1</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>31.3</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>31.3</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>32.4</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>32.4</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>33.1</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>33.1</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>34.200000000000003</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>34.200000000000003</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>35.1</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>35.200000000000003</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>36.1</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>36.200000000000003</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>1795</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>36.200000000000003</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>36.299999999999997</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>36.299999999999997</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>37.1</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>37.1</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>38.299999999999997</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>38.299999999999997</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>39.4</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>39.4</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>40.200000000000003</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>40.200000000000003</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>40.299999999999997</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>41.3</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>41.3</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>42.3</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>42.3</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>43.1</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>43.1</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>43.2</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>43.2</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>44.2</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>44.2</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <v>45.1</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>47.1</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>47.1</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>48.2</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>48.2</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>48.2</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>49.3</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>49.3</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>50.2</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>51.1</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>51.1</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>52.1</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>52.1</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>52.3</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>52.3</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>53.4</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>53.4</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>54.4</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>55.2</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>55.2</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>56.2</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>58.2</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>58.2</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>59.2</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>59.2</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>60.2</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>60.2</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>61.3</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>62.1</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>65.099999999999994</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>65.099999999999994</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>66.099999999999994</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>66.099999999999994</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>1805</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>70.3</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>71.099999999999994</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>71.2</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>72.400000000000006</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>72.400000000000006</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>75.400000000000006</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>76.3</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>76.3</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>77.099999999999994</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>78.2</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>78.2</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>79.2</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>79.2</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>81.2</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>81.2</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>83.2</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>84.3</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>87.2</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>87.2</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>88.1</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A122" s="3">
         <v>88.1</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A123" s="3">
         <v>88.2</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A124" s="3">
         <v>90.1</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A125" s="3">
         <v>90.1</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="3">
         <v>91.1</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="3">
         <v>91.1</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A128" s="3">
         <v>92.1</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>92.1</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>93.1</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>93.1</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>94.2</v>
       </c>
@@ -5521,7 +5521,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>94.2</v>
       </c>
@@ -5559,7 +5559,7 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>94.4</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>96.2</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A136" s="3">
         <v>96.2</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>97.1</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A138" s="3">
         <v>97.1</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>98.1</v>
       </c>
@@ -5787,7 +5787,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A140" s="3">
         <v>100.1</v>
       </c>
@@ -5825,7 +5825,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>100.2</v>
       </c>
@@ -5863,7 +5863,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A142" s="3">
         <v>101.4</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A143" s="3">
         <v>101.4</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A144" s="3">
         <v>102.2</v>
       </c>
@@ -5977,7 +5977,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A145" s="3">
         <v>102.2</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
         <v>105.1</v>
       </c>
@@ -6053,7 +6053,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
         <v>105.1</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A148" s="3">
         <v>106.2</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
         <v>106.2</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" s="3">
         <v>107.3</v>
       </c>
@@ -6205,7 +6205,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
         <v>107.3</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A152" s="3">
         <v>110.2</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
         <v>110.2</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>110.3</v>
       </c>
@@ -6357,7 +6357,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>110.3</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A156" s="3">
         <v>110.4</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A157" s="3">
         <v>110.4</v>
       </c>
@@ -6471,7 +6471,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A158" s="3">
         <v>112.4</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
         <v>112.4</v>
       </c>
@@ -6547,7 +6547,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A160" s="3">
         <v>113.2</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" s="3">
         <v>113.2</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" s="3">
         <v>114.2</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" s="3">
         <v>117.3</v>
       </c>
@@ -6699,7 +6699,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164" s="3">
         <v>119.2</v>
       </c>
@@ -6737,7 +6737,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165" s="3">
         <v>119.2</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166" s="3">
         <v>120.3</v>
       </c>
@@ -6813,7 +6813,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A167" s="3">
         <v>120.3</v>
       </c>
@@ -6851,7 +6851,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A168" s="3">
         <v>121.2</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A169" s="3">
         <v>121.2</v>
       </c>
@@ -6927,7 +6927,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
         <v>123.4</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A171" s="3">
         <v>123.4</v>
       </c>
@@ -7003,7 +7003,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172" s="3">
         <v>126.1</v>
       </c>
@@ -7041,7 +7041,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173" s="3">
         <v>127.3</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A174" s="3">
         <v>127.3</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" s="3">
         <v>128.1</v>
       </c>
@@ -7155,7 +7155,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A176" s="3">
         <v>128.1</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A177" s="3">
         <v>129.1</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A178" s="3">
         <v>129.1</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A179" s="3">
         <v>129.30000000000001</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A180" s="3">
         <v>129.4</v>
       </c>
@@ -7345,7 +7345,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A181" s="3">
         <v>129.4</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" s="3">
         <v>130.19999999999999</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A183" s="3">
         <v>130.19999999999999</v>
       </c>
@@ -7459,7 +7459,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A184" s="3">
         <v>131.4</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A185" s="3">
         <v>131.4</v>
       </c>
@@ -7535,7 +7535,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A186" s="3">
         <v>132.19999999999999</v>
       </c>
@@ -7573,7 +7573,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A187" s="3">
         <v>132.19999999999999</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188" s="3">
         <v>133.1</v>
       </c>
@@ -7649,7 +7649,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A189" s="3">
         <v>133.1</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A190" s="3">
         <v>135.4</v>
       </c>
@@ -7725,7 +7725,7 @@
         <v>2425</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A191" s="3">
         <v>138.1</v>
       </c>
@@ -7763,7 +7763,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A192" s="3">
         <v>138.1</v>
       </c>
@@ -7801,7 +7801,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193" s="3">
         <v>139.1</v>
       </c>
@@ -7839,7 +7839,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194" s="3">
         <v>143.19999999999999</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195" s="3">
         <v>143.30000000000001</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A196" s="3">
         <v>144.1</v>
       </c>
@@ -7953,7 +7953,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A197" s="3">
         <v>144.1</v>
       </c>
@@ -7991,7 +7991,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A198" s="3">
         <v>144.30000000000001</v>
       </c>
@@ -8029,7 +8029,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199" s="3">
         <v>146.30000000000001</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A200" s="3">
         <v>146.30000000000001</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201" s="3">
         <v>147.30000000000001</v>
       </c>
@@ -8143,7 +8143,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A202" s="3">
         <v>147.30000000000001</v>
       </c>
@@ -8181,7 +8181,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A203" s="3">
         <v>148.1</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A204" s="3">
         <v>149.30000000000001</v>
       </c>
@@ -8257,7 +8257,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A205" s="3">
         <v>149.30000000000001</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206" s="3">
         <v>149.4</v>
       </c>
@@ -8333,7 +8333,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207" s="3">
         <v>149.4</v>
       </c>
@@ -8371,7 +8371,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208" s="3">
         <v>150.1</v>
       </c>
@@ -8409,7 +8409,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A209" s="3">
         <v>150.1</v>
       </c>
@@ -8447,7 +8447,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A210" s="3">
         <v>152.1</v>
       </c>
@@ -8485,7 +8485,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A211" s="3">
         <v>152.1</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A212" s="3">
         <v>153.19999999999999</v>
       </c>
@@ -8561,7 +8561,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A213" s="3">
         <v>153.19999999999999</v>
       </c>
@@ -8599,7 +8599,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A214" s="3">
         <v>154.19999999999999</v>
       </c>
@@ -8637,7 +8637,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A215" s="3">
         <v>154.19999999999999</v>
       </c>
@@ -8675,7 +8675,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A216" s="3">
         <v>155.1</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A217" s="3">
         <v>155.1</v>
       </c>
@@ -8751,7 +8751,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A218" s="3">
         <v>156.1</v>
       </c>
@@ -8789,7 +8789,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A219" s="3">
         <v>156.1</v>
       </c>
@@ -8827,7 +8827,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A220" s="3">
         <v>157.19999999999999</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>920.00000000000011</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A221" s="3">
         <v>158.1</v>
       </c>
@@ -8903,7 +8903,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222" s="3">
         <v>158.1</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" s="3">
         <v>158.19999999999999</v>
       </c>
@@ -8979,7 +8979,7 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A224" s="3">
         <v>158.30000000000001</v>
       </c>
@@ -9017,7 +9017,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A225" s="3">
         <v>158.30000000000001</v>
       </c>
@@ -9055,7 +9055,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A226" s="3">
         <v>160.19999999999999</v>
       </c>
@@ -9093,7 +9093,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A227" s="3">
         <v>160.19999999999999</v>
       </c>
@@ -9131,7 +9131,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A228" s="3">
         <v>161.1</v>
       </c>
@@ -9169,7 +9169,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A229" s="3">
         <v>161.19999999999999</v>
       </c>
@@ -9207,7 +9207,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A230" s="3">
         <v>161.19999999999999</v>
       </c>
@@ -9245,7 +9245,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A231" s="3">
         <v>2.2999999999999998</v>
       </c>
@@ -9283,7 +9283,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A232" s="3">
         <v>2.2999999999999998</v>
       </c>
@@ -9321,7 +9321,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A233" s="3">
         <v>2.2999999999999998</v>
       </c>
@@ -9359,7 +9359,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A234" s="3">
         <v>5.3</v>
       </c>
@@ -9397,7 +9397,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A235" s="3">
         <v>18.100000000000001</v>
       </c>
@@ -9435,7 +9435,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A236" s="3">
         <v>26.2</v>
       </c>
@@ -9473,7 +9473,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A237" s="3">
         <v>26.2</v>
       </c>
@@ -9511,7 +9511,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A238" s="3">
         <v>37.200000000000003</v>
       </c>
@@ -9549,7 +9549,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A239" s="3">
         <v>37.200000000000003</v>
       </c>
@@ -9587,7 +9587,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A240" s="3">
         <v>38.200000000000003</v>
       </c>
@@ -9625,7 +9625,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A241" s="3">
         <v>38.200000000000003</v>
       </c>
@@ -9663,7 +9663,7 @@
         <v>3260</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A242" s="3">
         <v>58.2</v>
       </c>
@@ -9701,7 +9701,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A243" s="3">
         <v>86.3</v>
       </c>
@@ -9739,7 +9739,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A244" s="3">
         <v>86.3</v>
       </c>
@@ -9777,7 +9777,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A245" s="3">
         <v>93.2</v>
       </c>
@@ -9815,7 +9815,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A246" s="3">
         <v>93.2</v>
       </c>
@@ -9853,7 +9853,7 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A247" s="3">
         <v>97.3</v>
       </c>
@@ -9891,7 +9891,7 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A248" s="3">
         <v>97.3</v>
       </c>
@@ -9929,7 +9929,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A249" s="3">
         <v>133.30000000000001</v>
       </c>
@@ -9967,7 +9967,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A250" s="3">
         <v>133.30000000000001</v>
       </c>
@@ -10005,7 +10005,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A251" s="3">
         <v>135.19999999999999</v>
       </c>
@@ -10043,7 +10043,7 @@
         <v>2165</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A252" s="3">
         <v>135.19999999999999</v>
       </c>
@@ -10081,7 +10081,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A253" s="3">
         <v>137.1</v>
       </c>
@@ -10119,7 +10119,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A254" s="3">
         <v>137.1</v>
       </c>
@@ -10157,7 +10157,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A255" s="3">
         <v>138.1</v>
       </c>
@@ -10195,7 +10195,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A256" s="3">
         <v>138.1</v>
       </c>
@@ -10233,7 +10233,7 @@
         <v>1455</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A257" s="3">
         <v>147.19999999999999</v>
       </c>
@@ -10271,7 +10271,7 @@
         <v>1930</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A258" s="3">
         <v>147.19999999999999</v>
       </c>
@@ -10309,7 +10309,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A259" s="3">
         <v>182.1</v>
       </c>
@@ -10347,7 +10347,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A260" s="3">
         <v>182.1</v>
       </c>
@@ -10385,7 +10385,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A261" s="3">
         <v>182.1</v>
       </c>
@@ -10423,7 +10423,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A262" s="3">
         <v>192.1</v>
       </c>
@@ -10461,7 +10461,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A263" s="3">
         <v>192.1</v>
       </c>
@@ -10499,7 +10499,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A264" s="3">
         <v>225.2</v>
       </c>
@@ -10537,7 +10537,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A265" s="3">
         <v>227.1</v>
       </c>
@@ -10575,7 +10575,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A266" s="3">
         <v>227.1</v>
       </c>
@@ -10613,7 +10613,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A267" s="3">
         <v>237.1</v>
       </c>
@@ -10651,7 +10651,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A268" s="3">
         <v>239.3</v>
       </c>
@@ -10689,7 +10689,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A269" s="3">
         <v>239.3</v>
       </c>
@@ -10727,7 +10727,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A270" s="3">
         <v>260.3</v>
       </c>
@@ -10765,7 +10765,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A271" s="3">
         <v>260.3</v>
       </c>
@@ -10803,7 +10803,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A272" s="3">
         <v>260.3</v>
       </c>
@@ -10841,7 +10841,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A273" s="3">
         <v>267.2</v>
       </c>
@@ -10879,7 +10879,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A274" s="3">
         <v>267.2</v>
       </c>
@@ -10917,7 +10917,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A275" s="3">
         <v>272.10000000000002</v>
       </c>
@@ -10955,7 +10955,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A276" s="3">
         <v>273.2</v>
       </c>
@@ -10993,7 +10993,7 @@
         <v>1530</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A277" s="3">
         <v>273.3</v>
       </c>
@@ -11031,7 +11031,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A278" s="3">
         <v>294.10000000000002</v>
       </c>
@@ -11069,7 +11069,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A279" s="3">
         <v>296.10000000000002</v>
       </c>
@@ -11107,7 +11107,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A280" s="3">
         <v>299.10000000000002</v>
       </c>
@@ -11145,7 +11145,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A281" s="3">
         <v>305.10000000000002</v>
       </c>
@@ -11183,7 +11183,7 @@
         <v>1940</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A282" s="3">
         <v>305.10000000000002</v>
       </c>
@@ -11221,7 +11221,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A283" s="3">
         <v>314.3</v>
       </c>
@@ -11259,7 +11259,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A284" s="3">
         <v>314.3</v>
       </c>
@@ -11297,7 +11297,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A285" s="3">
         <v>320.39999999999998</v>
       </c>
@@ -11335,7 +11335,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A286" s="3">
         <v>320.39999999999998</v>
       </c>
@@ -11373,7 +11373,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A287" s="3">
         <v>320.39999999999998</v>
       </c>
@@ -11411,7 +11411,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A288" s="3">
         <v>324.10000000000002</v>
       </c>
@@ -11449,7 +11449,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A289" s="3">
         <v>324.10000000000002</v>
       </c>
@@ -11487,7 +11487,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A290" s="3">
         <v>324.2</v>
       </c>
@@ -11525,7 +11525,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A291" s="3">
         <v>324.2</v>
       </c>
@@ -11563,7 +11563,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A292" s="3">
         <v>331.1</v>
       </c>
@@ -11601,7 +11601,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A293" s="3">
         <v>331.2</v>
       </c>
@@ -11639,7 +11639,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A294" s="3">
         <v>331.2</v>
       </c>
@@ -11677,7 +11677,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A295" s="3">
         <v>332.2</v>
       </c>
@@ -11715,7 +11715,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A296" s="3">
         <v>332.2</v>
       </c>
@@ -11753,7 +11753,7 @@
         <v>2485</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A297" s="3">
         <v>335.2</v>
       </c>
@@ -11791,7 +11791,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A298" s="3">
         <v>335.2</v>
       </c>
@@ -11829,7 +11829,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A299" s="3">
         <v>340.1</v>
       </c>
@@ -11867,7 +11867,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A300" s="3">
         <v>340.1</v>
       </c>
@@ -11905,7 +11905,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A301" s="5">
         <v>340.2</v>
       </c>
@@ -11943,7 +11943,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A302" s="5">
         <v>340.2</v>
       </c>
@@ -11981,7 +11981,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A303" s="3">
         <v>340.3</v>
       </c>
@@ -12019,7 +12019,7 @@
         <v>929.99999999999989</v>
       </c>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A304" s="3">
         <v>347.1</v>
       </c>
@@ -12057,7 +12057,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A305" s="3">
         <v>347.1</v>
       </c>
@@ -12095,7 +12095,7 @@
         <v>3670</v>
       </c>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A306" s="3">
         <v>358.3</v>
       </c>
@@ -12133,7 +12133,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A307" s="3">
         <v>361.2</v>
       </c>
@@ -12171,7 +12171,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A308" s="3">
         <v>361.2</v>
       </c>
@@ -12209,7 +12209,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A309" s="3">
         <v>384.2</v>
       </c>
@@ -12247,7 +12247,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A310" s="3">
         <v>384.2</v>
       </c>
@@ -12285,7 +12285,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A311" s="3">
         <v>390.4</v>
       </c>
@@ -12323,7 +12323,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A312" s="3">
         <v>390.4</v>
       </c>
@@ -12361,7 +12361,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A313" s="3">
         <v>392.2</v>
       </c>
@@ -12399,7 +12399,7 @@
         <v>2535</v>
       </c>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A314" s="3">
         <v>393.2</v>
       </c>
@@ -12437,7 +12437,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A315" s="3">
         <v>393.2</v>
       </c>
@@ -12475,7 +12475,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A316" s="3">
         <v>394.1</v>
       </c>
@@ -12513,7 +12513,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A317" s="3">
         <v>396.1</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>2980</v>
       </c>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A318" s="3">
         <v>396.1</v>
       </c>
@@ -12589,7 +12589,7 @@
         <v>2415</v>
       </c>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A319" s="3">
         <v>401.2</v>
       </c>
@@ -12627,7 +12627,7 @@
         <v>2695</v>
       </c>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A320" s="3">
         <v>401.1</v>
       </c>
@@ -12665,7 +12665,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A321" s="3">
         <v>401.1</v>
       </c>
@@ -12703,7 +12703,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A322" s="3">
         <v>404.3</v>
       </c>
@@ -12741,7 +12741,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A323" s="3">
         <v>404.3</v>
       </c>
@@ -12779,7 +12779,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A324" s="3">
         <v>407.1</v>
       </c>
@@ -12817,7 +12817,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A325" s="3">
         <v>409.1</v>
       </c>
@@ -12855,7 +12855,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A326" s="3">
         <v>409.1</v>
       </c>
@@ -12893,7 +12893,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A327" s="5">
         <v>409.3</v>
       </c>
@@ -12931,7 +12931,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A328" s="3">
         <v>416.3</v>
       </c>
@@ -12969,7 +12969,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A329" s="3">
         <v>420.1</v>
       </c>
@@ -13007,7 +13007,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A330" s="3">
         <v>420.1</v>
       </c>
@@ -13045,7 +13045,7 @@
         <v>2755</v>
       </c>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A331" s="3">
         <v>423.1</v>
       </c>
@@ -13083,7 +13083,7 @@
         <v>2615</v>
       </c>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A332" s="3">
         <v>429.1</v>
       </c>
@@ -13121,7 +13121,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A333" s="3">
         <v>432.2</v>
       </c>
@@ -13159,7 +13159,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A334" s="5">
         <v>432.3</v>
       </c>
@@ -13197,7 +13197,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A335" s="3">
         <v>438.1</v>
       </c>
@@ -13235,7 +13235,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A336" s="3">
         <v>438.1</v>
       </c>
@@ -13273,7 +13273,7 @@
         <v>1680.0000000000002</v>
       </c>
     </row>
-    <row r="337" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A337" s="3">
         <v>438.1</v>
       </c>
@@ -13311,7 +13311,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A338" s="3">
         <v>446.1</v>
       </c>
@@ -13349,7 +13349,7 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="339" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A339" s="3">
         <v>446.2</v>
       </c>
@@ -13387,7 +13387,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="340" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A340" s="3">
         <v>450.1</v>
       </c>
@@ -13425,7 +13425,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="341" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A341" s="3">
         <v>450.1</v>
       </c>
@@ -13463,7 +13463,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A342" s="3">
         <v>450.2</v>
       </c>
@@ -13501,7 +13501,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="343" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A343" s="3">
         <v>450.2</v>
       </c>
@@ -13539,7 +13539,7 @@
         <v>2485</v>
       </c>
     </row>
-    <row r="344" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A344" s="3">
         <v>463.2</v>
       </c>
@@ -13577,7 +13577,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="345" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A345" s="3">
         <v>463.2</v>
       </c>
@@ -13615,7 +13615,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="346" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A346" s="3">
         <v>475.3</v>
       </c>
@@ -13653,7 +13653,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="347" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A347" s="3">
         <v>475.3</v>
       </c>
@@ -13691,7 +13691,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="348" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A348" s="3">
         <v>475.3</v>
       </c>
@@ -13729,7 +13729,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="349" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A349" s="3">
         <v>476.1</v>
       </c>
@@ -13767,7 +13767,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="350" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A350" s="3">
         <v>476.1</v>
       </c>
@@ -13805,7 +13805,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="351" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A351" s="3">
         <v>476.1</v>
       </c>
@@ -13843,7 +13843,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="352" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A352" s="3">
         <v>476.3</v>
       </c>
@@ -13881,7 +13881,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="353" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A353" s="3">
         <v>476.3</v>
       </c>
@@ -13919,7 +13919,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A354" s="3">
         <v>476.3</v>
       </c>
@@ -13957,7 +13957,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="355" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A355" s="3">
         <v>481.1</v>
       </c>
@@ -13995,7 +13995,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="356" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A356" s="3">
         <v>481.1</v>
       </c>
@@ -14033,7 +14033,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A357" s="3">
         <v>481.1</v>
       </c>
@@ -14071,7 +14071,7 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A358" s="3">
         <v>487.2</v>
       </c>
@@ -14109,7 +14109,7 @@
         <v>1455</v>
       </c>
     </row>
-    <row r="359" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A359" s="3">
         <v>487.2</v>
       </c>
@@ -14147,7 +14147,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="360" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A360" s="3">
         <v>495.1</v>
       </c>
@@ -14185,7 +14185,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A361" s="3">
         <v>495.3</v>
       </c>
@@ -14223,7 +14223,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A362" s="3">
         <v>495.3</v>
       </c>
@@ -14261,7 +14261,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="363" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A363" s="3">
         <v>495.3</v>
       </c>
@@ -14299,7 +14299,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="364" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A364" s="3">
         <v>496.1</v>
       </c>
@@ -14337,7 +14337,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A365" s="3">
         <v>497.3</v>
       </c>
@@ -14375,7 +14375,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A366" s="3">
         <v>497.3</v>
       </c>
@@ -14413,7 +14413,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="367" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A367" s="3">
         <v>498.3</v>
       </c>
@@ -14451,7 +14451,7 @@
         <v>2350</v>
       </c>
     </row>
-    <row r="368" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A368" s="3">
         <v>500.1</v>
       </c>
@@ -14489,7 +14489,7 @@
         <v>2540</v>
       </c>
     </row>
-    <row r="369" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A369" s="3">
         <v>502.2</v>
       </c>
@@ -14527,7 +14527,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="370" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A370" s="3">
         <v>502.2</v>
       </c>
@@ -14565,7 +14565,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="371" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A371" s="3">
         <v>504.1</v>
       </c>
@@ -14603,7 +14603,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="372" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A372" s="3">
         <v>504.3</v>
       </c>
@@ -14641,7 +14641,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="373" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A373" s="3">
         <v>508.2</v>
       </c>
@@ -14679,7 +14679,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="374" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A374" s="3">
         <v>518.1</v>
       </c>
@@ -14717,7 +14717,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A375" s="3">
         <v>518.1</v>
       </c>
@@ -14755,7 +14755,7 @@
         <v>2340</v>
       </c>
     </row>
-    <row r="376" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A376" s="3">
         <v>518.20000000000005</v>
       </c>
@@ -14793,7 +14793,7 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="377" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A377" s="3">
         <v>518.20000000000005</v>
       </c>
@@ -14831,7 +14831,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A378" s="3">
         <v>524.1</v>
       </c>
@@ -14869,7 +14869,7 @@
         <v>1510</v>
       </c>
     </row>
-    <row r="379" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A379" s="3">
         <v>531.1</v>
       </c>
@@ -14907,7 +14907,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="380" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A380" s="3">
         <v>531.1</v>
       </c>
@@ -14945,7 +14945,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="381" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A381" s="3">
         <v>531.1</v>
       </c>
@@ -14983,7 +14983,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="382" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A382" s="3">
         <v>537.1</v>
       </c>
@@ -15021,7 +15021,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="383" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A383" s="3">
         <v>563.4</v>
       </c>
@@ -15059,7 +15059,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="384" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A384" s="3">
         <v>563.4</v>
       </c>
@@ -15097,7 +15097,7 @@
         <v>2440</v>
       </c>
     </row>
-    <row r="385" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A385" s="3">
         <v>565.1</v>
       </c>

</xml_diff>